<commit_message>
Maps markers can now be update using excel data
</commit_message>
<xml_diff>
--- a/assets/kerala-coordinates.xlsx
+++ b/assets/kerala-coordinates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Project-ELON\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47A36FF-B747-422B-BB6D-65BF036699B9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B15E50-D2AE-4687-9706-ECE2EC00C1C2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{7D583CA2-DDC8-492D-80CF-30AB18DB5588}"/>
   </bookViews>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67599973-629A-4947-B157-04537D600881}">
   <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,7 +669,7 @@
         <v>57</v>
       </c>
       <c r="E1">
-        <v>9.8214000000000006</v>
+        <v>9.6666000000000007</v>
       </c>
       <c r="F1">
         <v>76.521799999999999</v>
@@ -728,6 +728,12 @@
       <c r="D4">
         <v>6</v>
       </c>
+      <c r="E4">
+        <v>9.8221000000000007</v>
+      </c>
+      <c r="F4">
+        <v>75.423400000000001</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -741,6 +747,12 @@
       </c>
       <c r="D5">
         <v>32</v>
+      </c>
+      <c r="E5">
+        <v>9.7653999999999996</v>
+      </c>
+      <c r="F5">
+        <v>76.504000000000005</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>